<commit_message>
moved from static methods to classes
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\programming\mailFolderParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E97342-1FFE-4E9D-B152-27C16702DE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB7BDBB-F40E-4955-9B99-A64727F0735E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>LOGIN:</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>БРАТ СЫН СВАТ</t>
+  </si>
+  <si>
+    <t>alex-borrow@mail.ru</t>
+  </si>
+  <si>
+    <t>eGeEVSckqkVGee8VwWvc</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,17 +421,25 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FDAE2EA2-69B1-4ABE-96D9-14ECA1F206C6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>